<commit_message>
feat: mejorar la visualización de activos al cambiar 'name' por 'full_name' en la tabla y actualizar la lógica de generación de cargadores para laptops en el seeder
</commit_message>
<xml_diff>
--- a/storage/app/assets.xlsx
+++ b/storage/app/assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cechriza\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209B2F78-5B1F-4DFF-998E-D059CF3CA98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6C94B3-B825-4583-B086-6F5C9F1D0AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{E9455EA6-309A-4CAE-A1B0-EDC3900A81FA}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E9455EA6-309A-4CAE-A1B0-EDC3900A81FA}"/>
   </bookViews>
   <sheets>
     <sheet name="CECH LIMA" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="500">
   <si>
     <t>NOMBRES</t>
   </si>
@@ -227,9 +227,6 @@
     <t>ATOCHE DIAZ</t>
   </si>
   <si>
-    <t>CARGADOR-PATCHCORD</t>
-  </si>
-  <si>
     <t>CHUQUISPUMA RAMON</t>
   </si>
   <si>
@@ -602,9 +599,6 @@
     <t>MANUEL ALFREDO</t>
   </si>
   <si>
-    <t>ARRIVASPLATA GUANILLO</t>
-  </si>
-  <si>
     <t>1DKTYY2</t>
   </si>
   <si>
@@ -794,12 +788,6 @@
     <t>FRETEL CAMPO</t>
   </si>
   <si>
-    <t>ANGELO CRISTHIAN</t>
-  </si>
-  <si>
-    <t>GERONIMO MEDRANO</t>
-  </si>
-  <si>
     <t>5CG6266Z45</t>
   </si>
   <si>
@@ -1088,9 +1076,6 @@
     <t>EDWARD JEREMY</t>
   </si>
   <si>
-    <t>LOPEZ URCOHUARANGA</t>
-  </si>
-  <si>
     <t>14-BS11LA</t>
   </si>
   <si>
@@ -1118,9 +1103,6 @@
     <t>EDDY CARLOS</t>
   </si>
   <si>
-    <t>JOSE EMANUEL</t>
-  </si>
-  <si>
     <t>JAIME ANTHONY</t>
   </si>
   <si>
@@ -1190,9 +1172,6 @@
     <t>DAVID ALFREDO</t>
   </si>
   <si>
-    <t>ORLANDO WILFREDO</t>
-  </si>
-  <si>
     <t>GIANCARLO</t>
   </si>
   <si>
@@ -1277,18 +1256,9 @@
     <t>PF3T3KAC</t>
   </si>
   <si>
-    <t>CARGADOR + FUNDA</t>
-  </si>
-  <si>
-    <t>CARGADOR + CABLE ETHERNET</t>
-  </si>
-  <si>
     <t>Latitude 5400</t>
   </si>
   <si>
-    <t>CARGADOR + MOUSE</t>
-  </si>
-  <si>
     <t>Lenovo</t>
   </si>
   <si>
@@ -1319,9 +1289,6 @@
     <t>K6NOGR05323024H</t>
   </si>
   <si>
-    <t>CARGADOR+ CABLE ETHERNET</t>
-  </si>
-  <si>
     <t>83A1</t>
   </si>
   <si>
@@ -1554,6 +1521,33 @@
   </si>
   <si>
     <t>i5-8500T</t>
+  </si>
+  <si>
+    <t>LOPEZ URCOHURANGA</t>
+  </si>
+  <si>
+    <t>ANGELO</t>
+  </si>
+  <si>
+    <t>GERONIMO</t>
+  </si>
+  <si>
+    <t>ARRIVASPLATA GUANILO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WILFREDO ORLANDO </t>
+  </si>
+  <si>
+    <t>JOSUE EMANUEL</t>
+  </si>
+  <si>
+    <t>CARGADOR,PATCHCORD</t>
+  </si>
+  <si>
+    <t>CARGADOR,MOUSE</t>
+  </si>
+  <si>
+    <t>CARGADOR,FUNDA</t>
   </si>
 </sst>
 </file>
@@ -1665,7 +1659,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1705,6 +1699,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1910,7 +1910,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1971,12 +1971,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1998,9 +1992,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2036,21 +2027,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="63">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2502,44 +2502,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -2765,16 +2727,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{048782A8-1709-494E-9294-B47F686F14F6}" name="Tabla1" displayName="Tabla1" ref="A1:N100" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65" totalsRowBorderDxfId="64">
-  <autoFilter ref="A1:N100" xr:uid="{048782A8-1709-494E-9294-B47F686F14F6}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="BM8VMV2"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{048782A8-1709-494E-9294-B47F686F14F6}" name="Tabla1" displayName="Tabla1" ref="A1:N100" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+  <autoFilter ref="A1:N100" xr:uid="{048782A8-1709-494E-9294-B47F686F14F6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N65">
-    <sortCondition sortBy="cellColor" ref="A1:A100" dxfId="63"/>
+    <sortCondition sortBy="cellColor" ref="A1:A100" dxfId="58"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{A5B24B35-4320-4082-A617-C4970937CEA5}" name="NOMBRES"/>
@@ -2797,10 +2753,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{80A219E3-F2BC-49DB-93AB-B078A1F0E118}" name="Tabla13" displayName="Tabla13" ref="A1:M102" totalsRowShown="0" headerRowDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{80A219E3-F2BC-49DB-93AB-B078A1F0E118}" name="Tabla13" displayName="Tabla13" ref="A1:M102" totalsRowShown="0" headerRowDxfId="57">
   <autoFilter ref="A1:M102" xr:uid="{80A219E3-F2BC-49DB-93AB-B078A1F0E118}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M102">
-    <sortCondition sortBy="cellColor" ref="A1:A102" dxfId="61"/>
+    <sortCondition sortBy="cellColor" ref="A1:A102" dxfId="56"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{9A65F2B1-112E-43F9-AB9D-764926F83199}" name="NOMBRES"/>
@@ -2822,14 +2778,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{93B2C754-B355-46EF-A2C2-1977F7E40287}" name="Tabla134" displayName="Tabla134" ref="A1:L117" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
-  <autoFilter ref="A1:L117" xr:uid="{93B2C754-B355-46EF-A2C2-1977F7E40287}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="BM8VMV2"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{93B2C754-B355-46EF-A2C2-1977F7E40287}" name="Tabla134" displayName="Tabla134" ref="A1:L117" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+  <autoFilter ref="A1:L117" xr:uid="{93B2C754-B355-46EF-A2C2-1977F7E40287}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{87B50938-5309-4A9E-9CFE-C21BCD3F4F61}" name="NOMBRES"/>
     <tableColumn id="2" xr3:uid="{93561E5C-3BDD-49D7-9DA8-AD282D35577E}" name="APELLIDOS"/>
@@ -2849,7 +2799,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00F5F584-872A-4EED-86E2-EF902D61E210}" name="Tabla5" displayName="Tabla5" ref="A1:I3" totalsRowShown="0" headerRowDxfId="56" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00F5F584-872A-4EED-86E2-EF902D61E210}" name="Tabla5" displayName="Tabla5" ref="A1:I3" totalsRowShown="0" headerRowDxfId="51" tableBorderDxfId="50">
   <autoFilter ref="A1:I3" xr:uid="{00F5F584-872A-4EED-86E2-EF902D61E210}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{44FB088F-BBF4-4F04-BC09-00722A46D3E7}" name="EQUIPO"/>
@@ -2867,7 +2817,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D4213773-B5E8-4DC5-A28F-C4BD1D18837D}" name="Tabla57" displayName="Tabla57" ref="A1:K2" totalsRowShown="0" headerRowDxfId="54" tableBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D4213773-B5E8-4DC5-A28F-C4BD1D18837D}" name="Tabla57" displayName="Tabla57" ref="A1:K2" totalsRowShown="0" headerRowDxfId="49" tableBorderDxfId="48">
   <autoFilter ref="A1:K2" xr:uid="{D4213773-B5E8-4DC5-A28F-C4BD1D18837D}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{F1CE37B0-EF7C-4305-9A32-C3F0B571054A}" name="EQUIPO"/>
@@ -2887,7 +2837,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F4E7E247-37E4-4F04-8B0B-A776347FF6CB}" name="Tabla4" displayName="Tabla4" ref="A1:I20" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F4E7E247-37E4-4F04-8B0B-A776347FF6CB}" name="Tabla4" displayName="Tabla4" ref="A1:I20" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45">
   <autoFilter ref="A1:I20" xr:uid="{F4E7E247-37E4-4F04-8B0B-A776347FF6CB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{53C7B63E-4260-42CB-890C-34B3EB585039}" name="EQUIPO"/>
@@ -3202,12 +3152,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7761B29A-5971-49DE-B10E-5797F40E0A99}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:N100"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A49" sqref="A49"/>
-      <selection pane="bottomLeft" activeCell="B125" sqref="B125"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3269,11 +3219,11 @@
         <v>12</v>
       </c>
       <c r="N1" s="39" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
@@ -3309,9 +3259,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
-        <v>372</v>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>366</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
@@ -3346,12 +3296,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
-        <v>371</v>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>365</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>15</v>
@@ -3363,13 +3313,13 @@
         <v>17</v>
       </c>
       <c r="F4" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" t="s">
         <v>89</v>
-      </c>
-      <c r="H4" t="s">
-        <v>90</v>
       </c>
       <c r="I4" t="s">
         <v>30</v>
@@ -3380,15 +3330,15 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="35" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
-        <v>365</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>359</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>15</v>
@@ -3397,43 +3347,43 @@
         <v>16</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="G5" s="4"/>
       <c r="J5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
-        <v>382</v>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>375</v>
       </c>
       <c r="B6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" s="15" t="s">
+      <c r="F6" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>132</v>
-      </c>
       <c r="H6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>22</v>
@@ -3441,12 +3391,12 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
-        <v>367</v>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>361</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>15</v>
@@ -3458,7 +3408,7 @@
         <v>39</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>41</v>
@@ -3470,56 +3420,56 @@
         <v>21</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>423</v>
+        <v>497</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
-        <v>358</v>
-      </c>
-      <c r="B8" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>352</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="44" t="s">
-        <v>444</v>
-      </c>
-      <c r="F8" s="49" t="s">
-        <v>445</v>
-      </c>
-      <c r="G8" s="44" t="s">
-        <v>446</v>
-      </c>
-      <c r="H8" s="43" t="s">
+      <c r="E8" s="42" t="s">
+        <v>433</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>434</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>435</v>
+      </c>
+      <c r="H8" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="44" t="s">
-        <v>447</v>
-      </c>
-      <c r="J8" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="I8" s="42" t="s">
+        <v>436</v>
+      </c>
+      <c r="J8" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="22"/>
-      <c r="N8" s="43"/>
-    </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
-        <v>363</v>
+      <c r="N8" s="41"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="48" t="s">
+        <v>357</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>15</v>
@@ -3531,7 +3481,7 @@
         <v>39</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>41</v>
@@ -3543,57 +3493,57 @@
         <v>21</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>409</v>
+        <v>499</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N9" s="34"/>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
-        <v>361</v>
-      </c>
-      <c r="B10" s="42" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="C10" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>166</v>
-      </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="44" t="s">
+      <c r="H10" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="44" t="s">
+      <c r="I10" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="44" t="s">
-        <v>410</v>
-      </c>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-    </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
-        <v>369</v>
+      <c r="J10" s="42" t="s">
+        <v>497</v>
+      </c>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
+        <v>363</v>
       </c>
       <c r="B11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>15</v>
@@ -3602,11 +3552,11 @@
         <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H11" t="s">
         <v>29</v>
@@ -3615,19 +3565,19 @@
         <v>30</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>410</v>
+        <v>497</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="14"/>
-      <c r="N11" s="51"/>
-    </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
-        <v>366</v>
+      <c r="N11" s="49"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
+        <v>360</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>15</v>
@@ -3636,13 +3586,13 @@
         <v>16</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
         <v>20</v>
@@ -3651,53 +3601,53 @@
         <v>21</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>412</v>
+        <v>498</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="46" t="s">
+        <v>346</v>
+      </c>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="48" t="s">
-        <v>351</v>
-      </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="N13" s="48" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
-        <v>352</v>
+      <c r="N13" s="46" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
+        <v>347</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="4"/>
@@ -3708,81 +3658,81 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
+        <v>349</v>
+      </c>
+      <c r="B15" s="41" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
-        <v>354</v>
-      </c>
-      <c r="B15" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="44" t="s">
+      <c r="C15" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44" t="s">
+      <c r="F15" s="42"/>
+      <c r="G15" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="43" t="s">
+      <c r="H15" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="43" t="s">
+      <c r="I15" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="44" t="s">
-        <v>410</v>
-      </c>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
+      <c r="J15" s="42" t="s">
+        <v>497</v>
+      </c>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
       <c r="M15" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="N15" s="43"/>
-    </row>
-    <row r="16" spans="1:14" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
-        <v>378</v>
-      </c>
-      <c r="B16" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="N15" s="41"/>
+    </row>
+    <row r="16" spans="1:14" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="43" t="s">
+        <v>372</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>406</v>
+      </c>
+      <c r="F16" s="47"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42" t="s">
+        <v>497</v>
+      </c>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="C16" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>416</v>
-      </c>
-      <c r="F16" s="49"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44" t="s">
-        <v>410</v>
-      </c>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="N16" s="43"/>
-    </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
-        <v>383</v>
+      <c r="N16" s="41"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
+        <v>376</v>
       </c>
       <c r="B17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>15</v>
@@ -3791,50 +3741,53 @@
         <v>16</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="4"/>
+      <c r="J17" t="s">
+        <v>22</v>
+      </c>
       <c r="M17" s="14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="43" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="B18" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="C18" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="C18" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="43" t="s">
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41" t="s">
+        <v>498</v>
+      </c>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="41"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43" t="s">
-        <v>412</v>
-      </c>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="43"/>
-    </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="B19" s="41" t="s">
         <v>156</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>157</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
@@ -3843,7 +3796,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="4"/>
@@ -3853,10 +3806,10 @@
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="N19" s="61"/>
-    </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="N19" s="58"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
         <v>31</v>
       </c>
       <c r="B20" t="s">
@@ -3890,12 +3843,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
-        <v>368</v>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="43" t="s">
+        <v>362</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>15</v>
@@ -3904,13 +3857,13 @@
         <v>16</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="G21" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="H21" t="s">
         <v>20</v>
@@ -3924,12 +3877,12 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
-        <v>353</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>348</v>
       </c>
       <c r="B22" t="s">
         <v>24</v>
@@ -3961,12 +3914,12 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" t="s">
         <v>161</v>
-      </c>
-      <c r="B23" t="s">
-        <v>162</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
@@ -3978,7 +3931,7 @@
         <v>33</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>35</v>
@@ -3993,15 +3946,15 @@
         <v>22</v>
       </c>
       <c r="M23" s="35" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
-        <v>387</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="44" t="s">
+        <v>380</v>
       </c>
       <c r="B24" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
@@ -4010,64 +3963,64 @@
         <v>25</v>
       </c>
       <c r="E24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="G24" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="H24" t="s">
         <v>20</v>
       </c>
       <c r="I24" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="J24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
-        <v>359</v>
-      </c>
-      <c r="B25" s="43" t="s">
+    <row r="25" spans="1:14" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="43" t="s">
+        <v>353</v>
+      </c>
+      <c r="B25" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="49" t="s">
+      <c r="E25" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="49" t="s">
+      <c r="F25" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="G25" s="49" t="s">
+      <c r="G25" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="44" t="s">
+      <c r="H25" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="I25" s="43" t="s">
+      <c r="I25" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="J25" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
+      <c r="J25" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
       <c r="M25" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="N25" s="43"/>
-    </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
+      <c r="N25" s="41"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="44" t="s">
         <v>51</v>
       </c>
       <c r="B26" t="s">
@@ -4103,12 +4056,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="45" t="s">
-        <v>360</v>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="43" t="s">
+        <v>354</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>15</v>
@@ -4120,7 +4073,7 @@
         <v>39</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>41</v>
@@ -4132,20 +4085,20 @@
         <v>21</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>423</v>
+        <v>497</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
-        <v>364</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="43" t="s">
+        <v>358</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>15</v>
@@ -4154,13 +4107,13 @@
         <v>38</v>
       </c>
       <c r="E28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="G28" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="H28" t="s">
         <v>29</v>
@@ -4174,15 +4127,15 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="46" t="s">
-        <v>375</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="44" t="s">
+        <v>369</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
@@ -4194,7 +4147,7 @@
         <v>39</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>41</v>
@@ -4206,18 +4159,18 @@
         <v>21</v>
       </c>
       <c r="J29" t="s">
+        <v>77</v>
+      </c>
+      <c r="M29" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="M29" s="35" t="s">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="43" t="s">
+        <v>373</v>
+      </c>
+      <c r="B30" s="34" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
-        <v>379</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>80</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>15</v>
@@ -4226,13 +4179,13 @@
         <v>16</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="H30" s="25" t="s">
         <v>29</v>
@@ -4246,15 +4199,15 @@
       <c r="K30" s="25"/>
       <c r="L30" s="25"/>
       <c r="M30" s="35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="43" t="s">
+        <v>350</v>
+      </c>
+      <c r="B31" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
-        <v>355</v>
-      </c>
-      <c r="B31" t="s">
-        <v>85</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>15</v>
@@ -4281,15 +4234,15 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
-        <v>376</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="43" t="s">
+        <v>370</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>15</v>
@@ -4298,13 +4251,13 @@
         <v>16</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H32" t="s">
         <v>20</v>
@@ -4318,12 +4271,12 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
-        <v>381</v>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="43" t="s">
+        <v>374</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>15</v>
@@ -4335,7 +4288,7 @@
         <v>39</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>41</v>
@@ -4352,12 +4305,12 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>167</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>168</v>
       </c>
       <c r="C34" t="s">
         <v>15</v>
@@ -4369,7 +4322,7 @@
         <v>26</v>
       </c>
       <c r="F34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>28</v>
@@ -4384,12 +4337,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="45" t="s">
-        <v>357</v>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="43" t="s">
+        <v>351</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>15</v>
@@ -4401,7 +4354,7 @@
         <v>39</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>41</v>
@@ -4418,15 +4371,15 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="43" t="s">
+        <v>356</v>
+      </c>
+      <c r="B36" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
-        <v>362</v>
-      </c>
-      <c r="B36" t="s">
-        <v>102</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>15</v>
@@ -4438,7 +4391,7 @@
         <v>39</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>41</v>
@@ -4455,15 +4408,15 @@
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="46" t="s">
-        <v>358</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="44" t="s">
+        <v>352</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
         <v>15</v>
@@ -4472,10 +4425,10 @@
         <v>25</v>
       </c>
       <c r="E37" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37" t="s">
         <v>111</v>
-      </c>
-      <c r="F37" t="s">
-        <v>112</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>48</v>
@@ -4492,15 +4445,15 @@
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="72" t="s">
+        <v>496</v>
+      </c>
+      <c r="B38" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="46" t="s">
-        <v>356</v>
-      </c>
-      <c r="B38" t="s">
-        <v>114</v>
       </c>
       <c r="C38" t="s">
         <v>15</v>
@@ -4512,7 +4465,7 @@
         <v>39</v>
       </c>
       <c r="F38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>41</v>
@@ -4529,15 +4482,15 @@
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="45" t="s">
-        <v>377</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="43" t="s">
+        <v>371</v>
       </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>15</v>
@@ -4546,31 +4499,31 @@
         <v>38</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H39" t="s">
         <v>29</v>
       </c>
       <c r="I39" t="s">
+        <v>134</v>
+      </c>
+      <c r="J39" t="s">
+        <v>22</v>
+      </c>
+      <c r="M39" s="14"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="43" t="s">
+        <v>367</v>
+      </c>
+      <c r="B40" t="s">
         <v>135</v>
-      </c>
-      <c r="J39" t="s">
-        <v>22</v>
-      </c>
-      <c r="M39" s="14"/>
-    </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="45" t="s">
-        <v>373</v>
-      </c>
-      <c r="B40" t="s">
-        <v>136</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>15</v>
@@ -4579,13 +4532,13 @@
         <v>16</v>
       </c>
       <c r="E40" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F40" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="G40" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="H40" t="s">
         <v>20</v>
@@ -4597,15 +4550,15 @@
         <v>22</v>
       </c>
       <c r="M40" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="50" t="s">
-        <v>380</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="73" t="s">
+        <v>495</v>
       </c>
       <c r="B41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>45</v>
@@ -4617,10 +4570,10 @@
         <v>46</v>
       </c>
       <c r="F41" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>20</v>
@@ -4634,12 +4587,12 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="45" t="s">
-        <v>370</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="43" t="s">
+        <v>364</v>
       </c>
       <c r="B42" t="s">
         <v>37</v>
@@ -4674,12 +4627,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="45" t="s">
-        <v>374</v>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="43" t="s">
+        <v>368</v>
       </c>
       <c r="B43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s">
         <v>15</v>
@@ -4691,7 +4644,7 @@
         <v>39</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>41</v>
@@ -4708,131 +4661,75 @@
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
       <c r="M43" s="14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="27"/>
     </row>
-    <row r="65" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="66" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="67" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="68" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="69" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="70" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="71" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="72" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="73" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="74" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="75" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="76" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="77" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="78" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="79" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="80" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="81" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="82" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="83" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="84" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="85" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="86" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="87" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="88" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="89" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="90" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="91" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="92" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="93" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="94" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="95" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="96" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="97" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="98" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="99" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="100" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="F3">
-    <cfRule type="duplicateValues" dxfId="48" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="duplicateValues" dxfId="46" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="duplicateValues" dxfId="45" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="duplicateValues" dxfId="44" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" dxfId="43" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="42" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="duplicateValues" dxfId="41" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="duplicateValues" dxfId="40" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="duplicateValues" dxfId="39" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F16">
-    <cfRule type="duplicateValues" dxfId="38" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="duplicateValues" dxfId="37" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="duplicateValues" dxfId="36" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="duplicateValues" dxfId="35" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="duplicateValues" dxfId="34" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="duplicateValues" dxfId="33" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="duplicateValues" dxfId="32" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="duplicateValues" dxfId="31" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="duplicateValues" dxfId="30" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="duplicateValues" dxfId="29" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="duplicateValues" dxfId="28" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="3"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" xr:uid="{49C3C192-6F1E-4E9D-A016-4A4A06A791EA}"/>
@@ -4879,7 +4776,7 @@
   <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4936,15 +4833,15 @@
         <v>12</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>187</v>
+      <c r="A2" s="43" t="s">
+        <v>185</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>15</v>
@@ -4953,10 +4850,10 @@
         <v>38</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>41</v>
@@ -4972,51 +4869,51 @@
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" s="23" t="s">
+      <c r="G3" s="11" t="s">
         <v>201</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="H3" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
-        <v>213</v>
-      </c>
-      <c r="B4" t="s">
-        <v>214</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>15</v>
@@ -5028,7 +4925,7 @@
         <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>41</v>
@@ -5045,11 +4942,11 @@
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
-        <v>308</v>
+      <c r="A5" s="43" t="s">
+        <v>304</v>
       </c>
       <c r="B5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -5058,25 +4955,25 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="G5" s="11"/>
       <c r="J5" t="s">
         <v>22</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" t="s">
         <v>178</v>
-      </c>
-      <c r="B6" t="s">
-        <v>179</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -5085,13 +4982,13 @@
         <v>38</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F6" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>181</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>20</v>
@@ -5104,15 +5001,15 @@
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
-        <v>271</v>
+      <c r="A7" s="43" t="s">
+        <v>267</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>15</v>
@@ -5124,7 +5021,7 @@
         <v>33</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>35</v>
@@ -5140,15 +5037,15 @@
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="14" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
-        <v>216</v>
+      <c r="A8" s="43" t="s">
+        <v>214</v>
       </c>
       <c r="B8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>15</v>
@@ -5157,10 +5054,10 @@
         <v>16</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="G8" s="4"/>
       <c r="I8" s="4"/>
@@ -5169,102 +5066,102 @@
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="M8" s="34"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
-        <v>295</v>
+      <c r="A9" s="43" t="s">
+        <v>291</v>
       </c>
       <c r="B9" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="G9" s="4"/>
       <c r="J9" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>297</v>
-      </c>
-      <c r="M9" s="51"/>
+        <v>293</v>
+      </c>
+      <c r="M9" s="49"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
-        <v>246</v>
+      <c r="A10" s="44" t="s">
+        <v>244</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="F10" s="56"/>
+        <v>404</v>
+      </c>
+      <c r="F10" s="53"/>
       <c r="G10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>423</v>
+        <v>497</v>
       </c>
       <c r="K10" s="4"/>
-      <c r="M10" s="51"/>
+      <c r="M10" s="49"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F11" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="G11" s="11" t="s">
         <v>201</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46" t="s">
-        <v>319</v>
+      <c r="A12" s="44" t="s">
+        <v>315</v>
       </c>
       <c r="B12" t="s">
         <v>58</v>
@@ -5276,11 +5173,11 @@
         <v>16</v>
       </c>
       <c r="E12"/>
-      <c r="F12" s="54" t="s">
-        <v>320</v>
+      <c r="F12" s="51" t="s">
+        <v>316</v>
       </c>
       <c r="G12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="H12" t="s">
         <v>20</v>
@@ -5293,16 +5190,16 @@
       </c>
       <c r="K12"/>
       <c r="L12" s="35" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="M12"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
-        <v>234</v>
+      <c r="A13" s="43" t="s">
+        <v>232</v>
       </c>
       <c r="B13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>15</v>
@@ -5314,7 +5211,7 @@
         <v>26</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>28</v>
@@ -5330,15 +5227,15 @@
       </c>
       <c r="K13" s="4"/>
       <c r="L13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
-        <v>248</v>
+      <c r="A14" s="70" t="s">
+        <v>492</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>249</v>
+        <v>493</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -5350,7 +5247,7 @@
         <v>39</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G14" t="s">
         <v>41</v>
@@ -5362,15 +5259,15 @@
         <v>21</v>
       </c>
       <c r="J14" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
-        <v>238</v>
+      <c r="A15" s="43" t="s">
+        <v>236</v>
       </c>
       <c r="B15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
@@ -5379,10 +5276,10 @@
         <v>38</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>41</v>
@@ -5398,15 +5295,15 @@
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="17" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
-        <v>228</v>
+      <c r="A16" s="43" t="s">
+        <v>226</v>
       </c>
       <c r="B16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -5415,13 +5312,13 @@
         <v>16</v>
       </c>
       <c r="E16" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>232</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>20</v>
@@ -5434,15 +5331,15 @@
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
-        <v>290</v>
+      <c r="A17" s="43" t="s">
+        <v>286</v>
       </c>
       <c r="B17" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>15</v>
@@ -5451,13 +5348,13 @@
         <v>38</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>20</v>
@@ -5470,15 +5367,15 @@
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="14" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
-        <v>264</v>
+      <c r="A18" s="43" t="s">
+        <v>260</v>
       </c>
       <c r="B18" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>15</v>
@@ -5487,10 +5384,10 @@
         <v>38</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>41</v>
@@ -5506,62 +5403,62 @@
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="14" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
-        <v>279</v>
+      <c r="A19" s="43" t="s">
+        <v>275</v>
       </c>
       <c r="B19" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>201</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="H19" t="s">
         <v>20</v>
       </c>
       <c r="I19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J19" t="s">
         <v>22</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
-        <v>268</v>
+      <c r="A20" s="43" t="s">
+        <v>264</v>
       </c>
       <c r="B20" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>35</v>
@@ -5578,11 +5475,11 @@
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
-        <v>219</v>
+      <c r="A21" s="43" t="s">
+        <v>217</v>
       </c>
       <c r="B21" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>15</v>
@@ -5591,7 +5488,7 @@
         <v>38</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="4" t="s">
@@ -5604,53 +5501,53 @@
         <v>21</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>59</v>
+        <v>497</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="52" t="s">
-        <v>305</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>306</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="40" t="s">
+      <c r="A22" s="75" t="s">
+        <v>301</v>
+      </c>
+      <c r="B22" s="76" t="s">
+        <v>302</v>
+      </c>
+      <c r="C22" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="F22" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="G22" s="40" t="s">
+      <c r="E22" s="74" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" s="74" t="s">
+        <v>303</v>
+      </c>
+      <c r="G22" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="40" t="s">
+      <c r="I22" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="40" t="s">
+      <c r="J22" s="74" t="s">
         <v>22</v>
       </c>
       <c r="K22" s="25"/>
       <c r="L22" s="34"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
-        <v>275</v>
+      <c r="A23" s="43" t="s">
+        <v>271</v>
       </c>
       <c r="B23" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>15</v>
@@ -5662,7 +5559,7 @@
         <v>26</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>28</v>
@@ -5678,18 +5575,18 @@
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="14" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
-        <v>252</v>
+      <c r="A24" s="44" t="s">
+        <v>248</v>
       </c>
       <c r="B24" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C24" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D24" t="s">
         <v>25</v>
@@ -5698,7 +5595,7 @@
         <v>33</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="G24" s="28" t="s">
         <v>35</v>
@@ -5714,11 +5611,11 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
-        <v>256</v>
+      <c r="A25" s="43" t="s">
+        <v>252</v>
       </c>
       <c r="B25" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>15</v>
@@ -5727,10 +5624,10 @@
         <v>38</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>41</v>
@@ -5746,15 +5643,15 @@
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
-        <v>286</v>
+      <c r="A26" s="43" t="s">
+        <v>282</v>
       </c>
       <c r="B26" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>45</v>
@@ -5766,10 +5663,10 @@
         <v>46</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H26" t="s">
         <v>20</v>
@@ -5778,31 +5675,31 @@
         <v>49</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>59</v>
+        <v>497</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="14" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="45" t="s">
-        <v>311</v>
+      <c r="A27" s="43" t="s">
+        <v>307</v>
       </c>
       <c r="B27" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C27" t="s">
         <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E27" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>35</v>
@@ -5819,11 +5716,11 @@
       <c r="K27" s="4"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="46" t="s">
-        <v>260</v>
+      <c r="A28" s="44" t="s">
+        <v>256</v>
       </c>
       <c r="B28" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C28" t="s">
         <v>15</v>
@@ -5835,7 +5732,7 @@
         <v>33</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="G28" s="28" t="s">
         <v>35</v>
@@ -5850,15 +5747,15 @@
         <v>22</v>
       </c>
       <c r="L28" s="35" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
-        <v>302</v>
+      <c r="A29" s="43" t="s">
+        <v>298</v>
       </c>
       <c r="B29" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>15</v>
@@ -5870,7 +5767,7 @@
         <v>39</v>
       </c>
       <c r="F29" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>41</v>
@@ -5887,11 +5784,11 @@
       <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
-        <v>222</v>
+      <c r="A30" s="44" t="s">
+        <v>220</v>
       </c>
       <c r="B30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
@@ -5903,7 +5800,7 @@
         <v>33</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G30" s="28" t="s">
         <v>35</v>
@@ -5919,11 +5816,11 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
-        <v>386</v>
+      <c r="A31" s="43" t="s">
+        <v>379</v>
       </c>
       <c r="B31" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>15</v>
@@ -5935,7 +5832,7 @@
         <v>39</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>41</v>
@@ -5951,15 +5848,15 @@
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="14" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="46" t="s">
-        <v>225</v>
+      <c r="A32" s="44" t="s">
+        <v>223</v>
       </c>
       <c r="B32" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C32" t="s">
         <v>15</v>
@@ -5971,7 +5868,7 @@
         <v>39</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>41</v>
@@ -5988,11 +5885,11 @@
       <c r="K32" s="4"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" t="s">
         <v>170</v>
-      </c>
-      <c r="B33" t="s">
-        <v>171</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>15</v>
@@ -6004,7 +5901,7 @@
         <v>39</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>41</v>
@@ -6020,15 +5917,15 @@
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
-        <v>183</v>
+      <c r="A34" s="71" t="s">
+        <v>182</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
+        <v>494</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>15</v>
@@ -6037,10 +5934,10 @@
         <v>25</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G34" s="19" t="s">
         <v>28</v>
@@ -6056,15 +5953,15 @@
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="45" t="s">
-        <v>242</v>
+      <c r="A35" s="43" t="s">
+        <v>240</v>
       </c>
       <c r="B35" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>15</v>
@@ -6076,7 +5973,7 @@
         <v>39</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>41</v>
@@ -6092,15 +5989,15 @@
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="14" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
-        <v>314</v>
+      <c r="A36" s="43" t="s">
+        <v>310</v>
       </c>
       <c r="B36" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>15</v>
@@ -6109,10 +6006,10 @@
         <v>38</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="F36" s="55" t="s">
-        <v>317</v>
+        <v>312</v>
+      </c>
+      <c r="F36" s="52" t="s">
+        <v>313</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>19</v>
@@ -6128,15 +6025,15 @@
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="14" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="45" t="s">
-        <v>205</v>
+      <c r="A37" s="43" t="s">
+        <v>203</v>
       </c>
       <c r="B37" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>15</v>
@@ -6148,7 +6045,7 @@
         <v>39</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>41</v>
@@ -6164,15 +6061,15 @@
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
-        <v>298</v>
+      <c r="A38" s="43" t="s">
+        <v>294</v>
       </c>
       <c r="B38" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>15</v>
@@ -6183,8 +6080,8 @@
       <c r="E38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F38" s="56" t="s">
-        <v>300</v>
+      <c r="F38" s="53" t="s">
+        <v>296</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>41</v>
@@ -6200,15 +6097,15 @@
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="14" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B39" t="s">
         <v>174</v>
-      </c>
-      <c r="B39" t="s">
-        <v>175</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>15</v>
@@ -6219,8 +6116,8 @@
       <c r="E39" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F39" s="56" t="s">
-        <v>176</v>
+      <c r="F39" s="53" t="s">
+        <v>175</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>41</v>
@@ -6236,15 +6133,15 @@
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="46" t="s">
-        <v>191</v>
+      <c r="A40" s="44" t="s">
+        <v>189</v>
       </c>
       <c r="B40" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C40" t="s">
         <v>15</v>
@@ -6253,91 +6150,91 @@
         <v>25</v>
       </c>
       <c r="E40" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F40" t="s">
+        <v>192</v>
+      </c>
+      <c r="G40" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="F40" t="s">
+      <c r="H40" t="s">
         <v>194</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="I40" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="H40" t="s">
+      <c r="J40" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L40" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="I40" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L40" s="35" t="s">
-        <v>198</v>
-      </c>
     </row>
     <row r="49" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="54"/>
+      <c r="F49" s="51"/>
     </row>
     <row r="72" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F72" s="54"/>
+      <c r="F72" s="51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="F4">
-    <cfRule type="duplicateValues" dxfId="27" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="duplicateValues" dxfId="26" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="duplicateValues" dxfId="25" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="duplicateValues" dxfId="24" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" dxfId="23" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="22" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="duplicateValues" dxfId="21" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="duplicateValues" dxfId="20" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="duplicateValues" dxfId="19" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="duplicateValues" dxfId="18" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="duplicateValues" dxfId="17" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="duplicateValues" dxfId="16" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="duplicateValues" dxfId="15" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="duplicateValues" dxfId="14" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="duplicateValues" dxfId="13" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="duplicateValues" dxfId="12" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="duplicateValues" dxfId="11" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="L5" r:id="rId1" xr:uid="{C97769CF-3044-42AD-8E73-0AAB929F2485}"/>
@@ -6380,10 +6277,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE95060-0F69-4C4A-A3AE-72A8B7704C13}">
   <sheetPr codeName="Hoja3"/>
-  <dimension ref="A1:L117"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J118" sqref="J118"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6437,33 +6334,33 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>323</v>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>319</v>
       </c>
       <c r="B2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>201</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>22</v>
@@ -6471,77 +6368,77 @@
       <c r="K2" s="4"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
-        <v>326</v>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>322</v>
       </c>
       <c r="B3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="59" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="H3" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" t="s">
         <v>330</v>
       </c>
-      <c r="B4" t="s">
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
         <v>331</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" t="s">
-        <v>121</v>
-      </c>
-      <c r="I4" t="s">
-        <v>334</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
-        <v>335</v>
-      </c>
       <c r="B5" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>15</v>
@@ -6550,20 +6447,23 @@
         <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="G5" s="4"/>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
-        <v>337</v>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>333</v>
       </c>
       <c r="B6" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>15</v>
@@ -6572,10 +6472,10 @@
         <v>38</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>41</v>
@@ -6591,44 +6491,44 @@
       </c>
       <c r="L6" s="14"/>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
-        <v>340</v>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>336</v>
       </c>
       <c r="B7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
-        <v>343</v>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>339</v>
       </c>
       <c r="B8" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>15</v>
@@ -6637,10 +6537,10 @@
         <v>16</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>19</v>
@@ -6649,18 +6549,18 @@
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="J8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
-        <v>345</v>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="72" t="s">
+        <v>341</v>
       </c>
       <c r="B9" t="s">
-        <v>346</v>
+        <v>491</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -6669,18 +6569,21 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>348</v>
+        <v>343</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
-        <v>128</v>
+      <c r="A10" s="43" t="s">
+        <v>127</v>
       </c>
       <c r="B10" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>15</v>
@@ -6692,7 +6595,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>35</v>
@@ -6704,243 +6607,140 @@
         <v>21</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>59</v>
+        <v>497</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>388</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>391</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>389</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>390</v>
+      </c>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
+        <v>388</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>391</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>393</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>394</v>
+      </c>
+      <c r="E12" s="41" t="s">
         <v>395</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="F12" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="44" t="s">
+        <v>392</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>399</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>389</v>
+      </c>
+      <c r="F13" s="60">
+        <v>8551705504</v>
+      </c>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
+        <v>392</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>399</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>393</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>394</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>397</v>
+      </c>
+      <c r="F14" s="41" t="s">
         <v>398</v>
       </c>
-      <c r="C11" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="43" t="s">
-        <v>396</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>397</v>
-      </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="43" t="s">
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46" t="s">
-        <v>395</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>398</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>400</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>401</v>
-      </c>
-      <c r="E12" s="43" t="s">
-        <v>402</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>403</v>
-      </c>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
-        <v>399</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>406</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="43" t="s">
-        <v>396</v>
-      </c>
-      <c r="F13" s="63">
-        <v>8551705504</v>
-      </c>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
-        <v>399</v>
-      </c>
-      <c r="B14" s="43" t="s">
-        <v>406</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>400</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>401</v>
-      </c>
-      <c r="E14" s="43" t="s">
-        <v>404</v>
-      </c>
-      <c r="F14" s="43" t="s">
-        <v>405</v>
-      </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="17" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="18" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="19" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="20" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="22" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="23" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="24" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="25" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="26" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="27" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="28" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="29" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="30" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="31" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="32" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="34" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="35" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="36" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="37" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="39" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="43" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="46" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="47" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="48" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="49" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="50" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="51" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="52" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="53" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="54" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="55" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="56" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="57" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="58" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="59" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="60" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="61" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="62" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="63" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="64" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="65" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="66" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="67" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="68" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="69" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="70" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="71" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="72" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="73" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="74" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="75" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="76" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="77" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="78" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="79" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="80" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="81" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="82" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="83" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="84" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="85" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="86" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="87" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="88" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="89" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="90" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="91" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="92" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="93" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="94" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="95" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="96" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="97" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="98" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="99" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="100" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="101" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="102" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="103" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="104" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="105" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="106" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="107" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="108" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="109" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="110" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="111" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="112" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="113" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="114" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="115" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="116" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="117" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="F3">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -6995,7 +6795,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="33" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7006,13 +6806,13 @@
         <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="D2" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="I2" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -7023,39 +6823,39 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="D3" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="I3" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="65" t="s">
+      <c r="A4" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="65" t="s">
-        <v>430</v>
-      </c>
-      <c r="D4" s="65" t="s">
-        <v>431</v>
-      </c>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65" t="s">
-        <v>432</v>
+      <c r="C4" s="62" t="s">
+        <v>419</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>420</v>
+      </c>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J12" s="65"/>
-      <c r="K12" s="66"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7112,13 +6912,13 @@
         <v>9</v>
       </c>
       <c r="I1" s="33" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="J1" s="33" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="K1" s="33" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7129,51 +6929,51 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="I2" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="J2" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="K2" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="70" t="s">
+      <c r="A3" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="70" t="s">
-        <v>484</v>
-      </c>
-      <c r="D3" s="70" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" s="70" t="s">
-        <v>485</v>
-      </c>
-      <c r="F3" s="70" t="s">
+      <c r="C3" s="67" t="s">
+        <v>473</v>
+      </c>
+      <c r="D3" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="67" t="s">
+        <v>474</v>
+      </c>
+      <c r="F3" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="70" t="s">
-        <v>486</v>
-      </c>
-      <c r="H3" s="70" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="70" t="s">
-        <v>487</v>
+      <c r="G3" s="67" t="s">
+        <v>475</v>
+      </c>
+      <c r="H3" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="67" t="s">
+        <v>476</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -7231,7 +7031,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -7242,19 +7042,19 @@
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>22</v>
@@ -7262,26 +7062,26 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="B3" s="71" t="s">
-        <v>491</v>
-      </c>
-      <c r="C3" s="72" t="s">
-        <v>492</v>
-      </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
+        <v>479</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>480</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>481</v>
+      </c>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -7292,49 +7092,49 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>29</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -7362,243 +7162,243 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
-        <v>480</v>
-      </c>
-      <c r="B1" s="68" t="s">
+      <c r="A1" s="64" t="s">
+        <v>469</v>
+      </c>
+      <c r="B1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="68" t="s">
-        <v>481</v>
-      </c>
-      <c r="E1" s="68" t="s">
-        <v>482</v>
-      </c>
-      <c r="F1" s="68" t="s">
-        <v>483</v>
+      <c r="D1" s="65" t="s">
+        <v>470</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>471</v>
+      </c>
+      <c r="F1" s="65" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="B2" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C2" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="D2" t="s">
-        <v>451</v>
-      </c>
-      <c r="E2" s="69">
+        <v>440</v>
+      </c>
+      <c r="E2" s="66">
         <v>664</v>
       </c>
       <c r="F2" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="D3" t="s">
-        <v>455</v>
-      </c>
-      <c r="E3" s="69" t="s">
-        <v>456</v>
+        <v>444</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>445</v>
       </c>
       <c r="F3" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="D4" t="s">
-        <v>455</v>
-      </c>
-      <c r="E4" s="69" t="s">
-        <v>458</v>
+        <v>444</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>447</v>
       </c>
       <c r="F4" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="D5" t="s">
-        <v>455</v>
-      </c>
-      <c r="E5" s="69" t="s">
-        <v>461</v>
+        <v>444</v>
+      </c>
+      <c r="E5" s="66" t="s">
+        <v>450</v>
       </c>
       <c r="F5" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="D6" t="s">
-        <v>455</v>
-      </c>
-      <c r="E6" s="69" t="s">
-        <v>464</v>
+        <v>444</v>
+      </c>
+      <c r="E6" s="66" t="s">
+        <v>453</v>
       </c>
       <c r="F6" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="B7" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C7" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
       <c r="D7" t="s">
-        <v>451</v>
-      </c>
-      <c r="E7" s="69">
+        <v>440</v>
+      </c>
+      <c r="E7" s="66">
         <v>544</v>
       </c>
       <c r="F7" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="B8" t="s">
         <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="D8" t="s">
-        <v>455</v>
-      </c>
-      <c r="E8" s="69" t="s">
-        <v>469</v>
+        <v>444</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>458</v>
       </c>
       <c r="F8" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="D9" t="s">
-        <v>451</v>
-      </c>
-      <c r="E9" s="69" t="s">
-        <v>472</v>
+        <v>440</v>
+      </c>
+      <c r="E9" s="66" t="s">
+        <v>461</v>
       </c>
       <c r="F9" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="B10" t="s">
         <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
       <c r="D10" t="s">
-        <v>455</v>
-      </c>
-      <c r="E10" s="69" t="s">
-        <v>476</v>
+        <v>444</v>
+      </c>
+      <c r="E10" s="66" t="s">
+        <v>465</v>
       </c>
       <c r="F10" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
       <c r="B11" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C11" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
       <c r="D11" t="s">
-        <v>455</v>
-      </c>
-      <c r="E11" s="69" t="s">
-        <v>479</v>
+        <v>444</v>
+      </c>
+      <c r="E11" s="66" t="s">
+        <v>468</v>
       </c>
       <c r="F11" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="D12" t="s">
-        <v>455</v>
-      </c>
-      <c r="E12" s="69" t="s">
-        <v>456</v>
+        <v>444</v>
+      </c>
+      <c r="E12" s="66" t="s">
+        <v>445</v>
       </c>
       <c r="F12" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -7616,6 +7416,19 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ccda677c-d47e-41e3-9f0f-bb7e9fe092aa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Responsable xmlns="ccda677c-d47e-41e3-9f0f-bb7e9fe092aa" xsi:nil="true"/>
+    <Fecha xmlns="ccda677c-d47e-41e3-9f0f-bb7e9fe092aa" xsi:nil="true"/>
+    <TaxCatchAll xmlns="7d884445-3d2b-4d2f-a5c8-52f2c582d699" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010053AD0A1E33F41645B7C17AA3FE2FDC7A" ma:contentTypeVersion="21" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="d3047d8b2c195696087e98843153f143">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ccda677c-d47e-41e3-9f0f-bb7e9fe092aa" xmlns:ns3="7d884445-3d2b-4d2f-a5c8-52f2c582d699" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f9fb659f12e922e720e9af332d44a36" ns2:_="" ns3:_="">
     <xsd:import namespace="ccda677c-d47e-41e3-9f0f-bb7e9fe092aa"/>
@@ -7890,19 +7703,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ccda677c-d47e-41e3-9f0f-bb7e9fe092aa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Responsable xmlns="ccda677c-d47e-41e3-9f0f-bb7e9fe092aa" xsi:nil="true"/>
-    <Fecha xmlns="ccda677c-d47e-41e3-9f0f-bb7e9fe092aa" xsi:nil="true"/>
-    <TaxCatchAll xmlns="7d884445-3d2b-4d2f-a5c8-52f2c582d699" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F158E06-BAB0-4893-91C7-AC2D0B102A6C}">
   <ds:schemaRefs>
@@ -7912,6 +7712,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{590544F1-C56B-4980-8803-5B1A718685B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="ccda677c-d47e-41e3-9f0f-bb7e9fe092aa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7d884445-3d2b-4d2f-a5c8-52f2c582d699"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A08F8860-4C76-4EF1-B3E0-9B345E1D4F41}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7928,21 +7745,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{590544F1-C56B-4980-8803-5B1A718685B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="ccda677c-d47e-41e3-9f0f-bb7e9fe092aa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7d884445-3d2b-4d2f-a5c8-52f2c582d699"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>